<commit_message>
updated mar goal with fishpond indicator
</commit_message>
<xml_diff>
--- a/prep/Sense of Place/sacred places.xlsx
+++ b/prep/Sense of Place/sacred places.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents and Settings\eschemmel\Documents\github\mhi\prep\Sense of Place\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="27795" windowHeight="10035"/>
+    <workbookView minimized="1" xWindow="360" yWindow="135" windowWidth="27795" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -78,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0\ \ \ \ \ \ \ \ \ "/>
     <numFmt numFmtId="165" formatCode="0\ \ \ \ \ \ \ \ \ \ \ "/>
@@ -285,6 +290,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -332,7 +340,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,9 +373,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,6 +425,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -578,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>